<commit_message>
using only AvesTables.xlsx to populate DB tables, bird familes are included there
</commit_message>
<xml_diff>
--- a/Extras/BirdFamilies.xlsx
+++ b/Extras/BirdFamilies.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
   <si>
     <t>Id</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Alaudidae</t>
   </si>
   <si>
-    <t>Auks</t>
-  </si>
-  <si>
     <t>Alcidae</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>Apodidae</t>
   </si>
   <si>
-    <t>Herons</t>
-  </si>
-  <si>
     <t>Ardeidae</t>
   </si>
   <si>
@@ -75,21 +69,12 @@
     <t>Burhinidae</t>
   </si>
   <si>
-    <t>Nightjars</t>
-  </si>
-  <si>
-    <t>Caprimuldidae</t>
-  </si>
-  <si>
     <t>Treekeepers</t>
   </si>
   <si>
     <t>Certhiidae</t>
   </si>
   <si>
-    <t>Plovers</t>
-  </si>
-  <si>
     <t>Charadriidae</t>
   </si>
   <si>
@@ -105,21 +90,12 @@
     <t>Cinclidae</t>
   </si>
   <si>
-    <t>Pigeons</t>
-  </si>
-  <si>
     <t>Columbidae</t>
   </si>
   <si>
-    <t>Coraciiformes</t>
-  </si>
-  <si>
     <t>Kingfishers and Allies</t>
   </si>
   <si>
-    <t>Crows</t>
-  </si>
-  <si>
     <t>Corvidae</t>
   </si>
   <si>
@@ -135,9 +111,6 @@
     <t>Emberizidae</t>
   </si>
   <si>
-    <t>Falcons</t>
-  </si>
-  <si>
     <t>Falconidae</t>
   </si>
   <si>
@@ -147,15 +120,9 @@
     <t>Fregatidae</t>
   </si>
   <si>
-    <t>Finches</t>
-  </si>
-  <si>
     <t>Fringillidae</t>
   </si>
   <si>
-    <t>Divers</t>
-  </si>
-  <si>
     <t>Gaviidae</t>
   </si>
   <si>
@@ -183,9 +150,6 @@
     <t>Swallows and Martins</t>
   </si>
   <si>
-    <t>New World Blackbirds</t>
-  </si>
-  <si>
     <t>Icteridae</t>
   </si>
   <si>
@@ -195,27 +159,15 @@
     <t>Laniidae</t>
   </si>
   <si>
-    <t>Gulls</t>
-  </si>
-  <si>
     <t>Laridae</t>
   </si>
   <si>
-    <t>Mockingbirds</t>
-  </si>
-  <si>
     <t>Mimidae</t>
   </si>
   <si>
-    <t>Wagtails</t>
-  </si>
-  <si>
     <t>Motacillidae</t>
   </si>
   <si>
-    <t>Flycatchers</t>
-  </si>
-  <si>
     <t>Muscicapidae</t>
   </si>
   <si>
@@ -231,9 +183,6 @@
     <t>Otididae</t>
   </si>
   <si>
-    <t>Tits</t>
-  </si>
-  <si>
     <t>Paridae</t>
   </si>
   <si>
@@ -243,9 +192,6 @@
     <t>Parulidae</t>
   </si>
   <si>
-    <t>Sparrows</t>
-  </si>
-  <si>
     <t>Passeridae</t>
   </si>
   <si>
@@ -261,9 +207,6 @@
     <t>Phaethontidae</t>
   </si>
   <si>
-    <t>Cormorants</t>
-  </si>
-  <si>
     <t>Phalacrocoridae</t>
   </si>
   <si>
@@ -300,9 +243,6 @@
     <t>Shearwaters and Petrels</t>
   </si>
   <si>
-    <t>Procellariformes</t>
-  </si>
-  <si>
     <t>Accentors</t>
   </si>
   <si>
@@ -321,9 +261,6 @@
     <t>Pteroclididae</t>
   </si>
   <si>
-    <t>Rails</t>
-  </si>
-  <si>
     <t>Rallidae</t>
   </si>
   <si>
@@ -336,18 +273,12 @@
     <t>Sandpipers ans Allies</t>
   </si>
   <si>
-    <t>Scolopacide</t>
-  </si>
-  <si>
     <t>Nuthatches</t>
   </si>
   <si>
     <t>Sittidae</t>
   </si>
   <si>
-    <t>Skuas</t>
-  </si>
-  <si>
     <t>Stercorariidae</t>
   </si>
   <si>
@@ -375,9 +306,6 @@
     <t>Sulidae</t>
   </si>
   <si>
-    <t>Warblers</t>
-  </si>
-  <si>
     <t>Sylviidae</t>
   </si>
   <si>
@@ -399,25 +327,232 @@
     <t>Troglodytidae</t>
   </si>
   <si>
-    <t>Chats</t>
-  </si>
-  <si>
     <t>Turdidae</t>
   </si>
   <si>
-    <t>Thrushes</t>
-  </si>
-  <si>
     <t>Tyrant Flycatchers</t>
   </si>
   <si>
     <t>Tyrannidae</t>
   </si>
   <si>
-    <t>Vireos</t>
-  </si>
-  <si>
     <t>Vireonidae</t>
+  </si>
+  <si>
+    <t>Guans, Chachalacas and Curassows</t>
+  </si>
+  <si>
+    <t>Cracidae</t>
+  </si>
+  <si>
+    <t>New World Quail</t>
+  </si>
+  <si>
+    <t>Odontophoridae</t>
+  </si>
+  <si>
+    <t>Pigeons and Doves</t>
+  </si>
+  <si>
+    <t>Caprimulgidae</t>
+  </si>
+  <si>
+    <t>Nightjars and Allies</t>
+  </si>
+  <si>
+    <t>Hummingbirds</t>
+  </si>
+  <si>
+    <t>Trochilidae</t>
+  </si>
+  <si>
+    <t>Rails, Gallinules and Coots</t>
+  </si>
+  <si>
+    <t>Limpkin</t>
+  </si>
+  <si>
+    <t>Aramidae</t>
+  </si>
+  <si>
+    <t>Plovers and Lapwings</t>
+  </si>
+  <si>
+    <t>Scolopacidae</t>
+  </si>
+  <si>
+    <t>Skuas and Jaegers</t>
+  </si>
+  <si>
+    <t>Auks, Murres and Puffins</t>
+  </si>
+  <si>
+    <t>Gulls, Terns and Skimmers</t>
+  </si>
+  <si>
+    <t>Loons</t>
+  </si>
+  <si>
+    <t>Albatrosses</t>
+  </si>
+  <si>
+    <t>Diomedeidae</t>
+  </si>
+  <si>
+    <t>Northern Storm-Petrels</t>
+  </si>
+  <si>
+    <t>Hydrobatidae</t>
+  </si>
+  <si>
+    <t>Procellariidae</t>
+  </si>
+  <si>
+    <t>Anhingas</t>
+  </si>
+  <si>
+    <t>Anhingidae</t>
+  </si>
+  <si>
+    <t>Cormorants and Shags</t>
+  </si>
+  <si>
+    <t>Herons, Egrets and Bitterns</t>
+  </si>
+  <si>
+    <t>Ibises and Spoonbills</t>
+  </si>
+  <si>
+    <t>Threskiornithidae</t>
+  </si>
+  <si>
+    <t>New World Vultures</t>
+  </si>
+  <si>
+    <t>Cathartidae</t>
+  </si>
+  <si>
+    <t>Osprey</t>
+  </si>
+  <si>
+    <t>Pandionidae</t>
+  </si>
+  <si>
+    <t>Barn-Owls</t>
+  </si>
+  <si>
+    <t>Tytonidae</t>
+  </si>
+  <si>
+    <t>Trogons</t>
+  </si>
+  <si>
+    <t>Trogonidae</t>
+  </si>
+  <si>
+    <t>Alcedinidae</t>
+  </si>
+  <si>
+    <t>Falcons and Caracaras</t>
+  </si>
+  <si>
+    <t>Vireos, Shrike-Babblers and Erpornis</t>
+  </si>
+  <si>
+    <t>Crows, Jays and Magpies</t>
+  </si>
+  <si>
+    <t>Tits, Chickadees and Titmice</t>
+  </si>
+  <si>
+    <t>Penduline-Tits</t>
+  </si>
+  <si>
+    <t>Remizidae</t>
+  </si>
+  <si>
+    <t>Leaf Warblers</t>
+  </si>
+  <si>
+    <t>Phylloscopidae</t>
+  </si>
+  <si>
+    <t>Long-tailed Tits</t>
+  </si>
+  <si>
+    <t>Aegithalidae</t>
+  </si>
+  <si>
+    <t>Sylviid Warblers, Parrotbills and Allies</t>
+  </si>
+  <si>
+    <t>Kinglets</t>
+  </si>
+  <si>
+    <t>Regulidae</t>
+  </si>
+  <si>
+    <t>Gnatcatchers</t>
+  </si>
+  <si>
+    <t>Polioptilidae</t>
+  </si>
+  <si>
+    <t>Mockingbirds and Thrashers</t>
+  </si>
+  <si>
+    <t>Thrushes and Allies</t>
+  </si>
+  <si>
+    <t>Old World Flycatchers</t>
+  </si>
+  <si>
+    <t>Silky-flycatchers</t>
+  </si>
+  <si>
+    <t>Ptiliogonatidae</t>
+  </si>
+  <si>
+    <t>Olive Warbler</t>
+  </si>
+  <si>
+    <t>Peucedramidae</t>
+  </si>
+  <si>
+    <t>Old World Sparrows</t>
+  </si>
+  <si>
+    <t>Wagtails and Pipits</t>
+  </si>
+  <si>
+    <t>Finches, Euphorias and Allies</t>
+  </si>
+  <si>
+    <t>Longspurs and Snow Buntings</t>
+  </si>
+  <si>
+    <t>Calcariidae</t>
+  </si>
+  <si>
+    <t>New World Sparrows</t>
+  </si>
+  <si>
+    <t>Passerellidae</t>
+  </si>
+  <si>
+    <t>Troupials and Allies</t>
+  </si>
+  <si>
+    <t>Yellow-breasted Chat</t>
+  </si>
+  <si>
+    <t>Icteriidae</t>
+  </si>
+  <si>
+    <t>Cardinals and Allies</t>
+  </si>
+  <si>
+    <t>Cardinalidae</t>
   </si>
 </sst>
 </file>
@@ -749,11 +884,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -789,10 +922,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -800,10 +933,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -811,10 +944,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -822,10 +955,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -833,10 +966,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -844,10 +977,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -855,10 +988,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -866,10 +999,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -877,10 +1010,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -888,10 +1021,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -899,10 +1032,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -910,10 +1043,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>170</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -921,10 +1054,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -932,10 +1065,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>177</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -943,10 +1076,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -954,10 +1087,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -965,10 +1098,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -976,10 +1109,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -987,10 +1120,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -998,10 +1131,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1009,10 +1142,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1020,10 +1153,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1031,10 +1164,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1042,10 +1175,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1053,10 +1186,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1064,10 +1197,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>145</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1075,10 +1208,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1086,10 +1219,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>169</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1097,10 +1230,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1108,10 +1241,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1119,10 +1252,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1130,10 +1263,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1141,10 +1274,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1152,10 +1285,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1163,10 +1296,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1174,10 +1307,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1185,10 +1318,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1196,10 +1329,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="C40" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1207,10 +1340,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>160</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1218,10 +1351,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>168</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1229,10 +1362,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>162</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1240,10 +1373,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="C44" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1251,10 +1384,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1262,10 +1395,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1273,10 +1406,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1284,10 +1417,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>148</v>
       </c>
       <c r="C48" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1295,10 +1428,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1306,10 +1439,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>172</v>
       </c>
       <c r="C50" t="s">
-        <v>100</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1317,10 +1450,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>167</v>
       </c>
       <c r="C51" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1328,10 +1461,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1339,10 +1472,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>165</v>
       </c>
       <c r="C53" t="s">
-        <v>106</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1350,10 +1483,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1361,10 +1494,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="C55" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1372,10 +1505,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1383,10 +1516,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="C57" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1394,10 +1527,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1405,10 +1538,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="C59" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1416,10 +1549,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="C60" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1427,10 +1560,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="C61" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1438,10 +1571,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="C62" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1449,10 +1582,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="C63" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1460,10 +1593,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s">
-        <v>128</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1471,10 +1604,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="C65" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1482,10 +1615,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="C66" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1493,10 +1626,252 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="C67" t="s">
-        <v>133</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>116</v>
+      </c>
+      <c r="C68" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>156</v>
+      </c>
+      <c r="C70" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>92</v>
+      </c>
+      <c r="C77" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>94</v>
+      </c>
+      <c r="C78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>155</v>
+      </c>
+      <c r="C79" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>97</v>
+      </c>
+      <c r="C80" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>99</v>
+      </c>
+      <c r="C81" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>134</v>
+      </c>
+      <c r="C82" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>114</v>
+      </c>
+      <c r="C83" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>101</v>
+      </c>
+      <c r="C84" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>142</v>
+      </c>
+      <c r="C85" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>161</v>
+      </c>
+      <c r="C86" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>104</v>
+      </c>
+      <c r="C87" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>140</v>
+      </c>
+      <c r="C88" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>146</v>
+      </c>
+      <c r="C89" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>